<commit_message>
PCB as ordered at JLCPCB
</commit_message>
<xml_diff>
--- a/pcb/sensactOutdoor/TPS92200.xlsx
+++ b/pcb/sensactOutdoor/TPS92200.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\sensact\pcb\sensactOutdoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7C9428-0E52-4FFB-BCCB-C85A95DE6AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD469F8-3A26-47BC-8F37-8A96D8A21723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="5340" windowWidth="28800" windowHeight="11900" xr2:uid="{336FBEF5-ACB0-403E-B2D6-D14185D505AF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{336FBEF5-ACB0-403E-B2D6-D14185D505AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>L</t>
   </si>
   <si>
-    <t>L_uF</t>
-  </si>
-  <si>
     <t>V_VB_REF</t>
   </si>
   <si>
@@ -66,6 +63,9 @@
   </si>
   <si>
     <t>V_IN_MAX</t>
+  </si>
+  <si>
+    <t>L_uH</t>
   </si>
 </sst>
 </file>
@@ -440,7 +440,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -459,7 +459,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>26.4</v>
@@ -508,7 +508,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <f>B9*1000000</f>
@@ -517,7 +517,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15">
         <v>9.9000000000000005E-2</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16">
         <f>B15/B4</f>

</xml_diff>